<commit_message>
Update question difficulty level
</commit_message>
<xml_diff>
--- a/question_difficulty_level_result/1.xlsx
+++ b/question_difficulty_level_result/1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F102"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,31 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>frequency</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>frequency_occurrence</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>frequency_occurrence_probab</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>max_probab</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>max_probab_percentage</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>recommended_level</t>
         </is>
       </c>
@@ -484,7 +509,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -514,7 +560,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>{"L3":7,"L2":1}</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>{"L3":0.875,"L2":0.125}</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>87.50</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -544,7 +611,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>8</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>{"L2":5,"L1":3}</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>{"L2":0.625,"L1":0.375}</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>62.50</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
@@ -574,7 +662,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="n">
+        <v>8</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>{"L3":6,"L2":2}</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>{"L3":0.75,"L2":0.25}</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>75.00</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -604,7 +713,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>{"L3":7,"L2":1}</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>{"L3":0.875,"L2":0.125}</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>87.50</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -634,7 +764,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -664,7 +815,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>{"L1":8}</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>{"L1":1.0}</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>L1</t>
         </is>
@@ -694,7 +866,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>{"L2":4,"L3":4}</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>{"L2":0.5,"L3":0.5}</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>50.00</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -724,7 +917,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>{"L3":7,"L2":1}</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>{"L3":0.875,"L2":0.125}</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>87.50</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -754,7 +968,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="n">
+        <v>8</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>{"L2":6,"L1":2}</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>{"L2":0.75,"L1":0.25}</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>75.00</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
@@ -784,7 +1019,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="n">
+        <v>8</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>{"L2":5,"L1":3}</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>{"L2":0.625,"L1":0.375}</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>62.50</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
@@ -814,7 +1070,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="n">
+        <v>8</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -844,7 +1121,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="n">
+        <v>8</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>{"L3":6,"L2":1,"L1":1}</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>{"L3":0.75,"L2":0.125,"L1":0.125}</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>75.00</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -874,7 +1172,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="n">
+        <v>8</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>{"L3":7,"L2":1}</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>{"L3":0.875,"L2":0.125}</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>87.50</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -904,7 +1223,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>{"L3":4,"L2":3,"L1":1}</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>{"L3":0.5,"L2":0.375,"L1":0.125}</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>50.00</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -934,7 +1274,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="n">
+        <v>8</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>{"L1":8}</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>{"L1":1.0}</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>L1</t>
         </is>
@@ -964,7 +1325,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="n">
+        <v>8</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>{"L2":5,"L3":3}</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>{"L2":0.625,"L3":0.375}</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>62.50</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -994,7 +1376,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="n">
+        <v>8</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>{"L1":5,"L2":3}</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>{"L1":0.625,"L2":0.375}</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>62.50</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
@@ -1024,7 +1427,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="n">
+        <v>8</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>{"L3":6,"L2":2}</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>{"L3":0.75,"L2":0.25}</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>75.00</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1054,7 +1478,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" t="n">
+        <v>8</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>{"L2":6,"L1":2}</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>{"L2":0.75,"L1":0.25}</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>75.00</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
@@ -1084,7 +1529,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" t="n">
+        <v>9</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>{"L3":8,"L1":1}</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>{"L3":0.8888888889,"L1":0.1111111111}</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>88.89</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1114,7 +1580,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F23" t="n">
+        <v>8</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>{"L3":7,"L2":1}</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>{"L3":0.875,"L2":0.125}</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>87.50</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1144,7 +1631,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F24" t="n">
+        <v>8</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>{"L3":6,"L1":2}</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>{"L3":0.75,"L1":0.25}</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>75.00</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1174,7 +1682,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" t="n">
+        <v>8</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1204,7 +1733,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F26" t="n">
+        <v>8</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1234,7 +1784,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="F27" t="n">
+        <v>8</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>{"L3":7,"L2":1}</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>{"L3":0.875,"L2":0.125}</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>87.50</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1264,7 +1835,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="F28" t="n">
+        <v>8</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>{"L3":7,"L2":1}</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>{"L3":0.875,"L2":0.125}</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>87.50</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1294,7 +1886,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F29" t="n">
+        <v>8</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>{"L2":4,"L3":3,"L1":1}</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>{"L2":0.5,"L3":0.375,"L1":0.125}</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>50.00</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1324,7 +1937,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="F30" t="n">
+        <v>8</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1354,7 +1988,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F31" t="n">
+        <v>8</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>{"L2":6,"L3":1,"L1":1}</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>{"L2":0.75,"L3":0.125,"L1":0.125}</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>75.00</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1384,7 +2039,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F32" t="n">
+        <v>8</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1414,7 +2090,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F33" t="n">
+        <v>8</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>{"L1":5,"L2":3}</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>{"L1":0.625,"L2":0.375}</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>62.50</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
@@ -1444,7 +2141,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="F34" t="n">
+        <v>8</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>{"L2":3,"L3":3,"L1":2}</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>{"L2":0.375,"L3":0.375,"L1":0.25}</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>37.50</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1474,7 +2192,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F35" t="n">
+        <v>8</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1504,7 +2243,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" t="n">
+        <v>8</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>{"L3":6,"L2":2}</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>{"L3":0.75,"L2":0.25}</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>75.00</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1534,7 +2294,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F37" t="n">
+        <v>8</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1564,7 +2345,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F38" t="n">
+        <v>8</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>{"L3":7,"L2":1}</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>{"L3":0.875,"L2":0.125}</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>87.50</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1594,7 +2396,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" t="n">
+        <v>8</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>{"L3":7,"L2":1}</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>{"L3":0.875,"L2":0.125}</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>87.50</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1624,7 +2447,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F40" t="n">
+        <v>8</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>{"L1":8}</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>{"L1":1.0}</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>1</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>L1</t>
         </is>
@@ -1654,7 +2498,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F41" t="n">
+        <v>8</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1684,7 +2549,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F42" t="n">
+        <v>8</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>{"L1":4,"L2":3,"L3":1}</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>{"L1":0.5,"L2":0.375,"L3":0.125}</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>50.00</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1714,7 +2600,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="F43" t="n">
+        <v>8</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>{"L1":8}</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>{"L1":1.0}</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>1</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
         <is>
           <t>L1</t>
         </is>
@@ -1744,7 +2651,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="F44" t="n">
+        <v>8</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>{"L1":4,"L2":4}</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>{"L1":0.5,"L2":0.5}</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>50.00</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
@@ -1774,7 +2702,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="F45" t="n">
+        <v>8</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>{"L3":8}</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
+        <v>1</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -1805,6 +2754,11 @@
         </is>
       </c>
       <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1831,6 +2785,11 @@
         </is>
       </c>
       <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1857,6 +2816,11 @@
         </is>
       </c>
       <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1883,6 +2847,11 @@
         </is>
       </c>
       <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1909,6 +2878,11 @@
         </is>
       </c>
       <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1935,6 +2909,11 @@
         </is>
       </c>
       <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1961,6 +2940,11 @@
         </is>
       </c>
       <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1987,6 +2971,11 @@
         </is>
       </c>
       <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2013,6 +3002,11 @@
         </is>
       </c>
       <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -2039,6 +3033,11 @@
         </is>
       </c>
       <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2065,6 +3064,11 @@
         </is>
       </c>
       <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2091,6 +3095,11 @@
         </is>
       </c>
       <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2117,6 +3126,11 @@
         </is>
       </c>
       <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2143,6 +3157,11 @@
         </is>
       </c>
       <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2169,6 +3188,11 @@
         </is>
       </c>
       <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2195,6 +3219,11 @@
         </is>
       </c>
       <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2221,6 +3250,11 @@
         </is>
       </c>
       <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2247,6 +3281,11 @@
         </is>
       </c>
       <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2273,6 +3312,11 @@
         </is>
       </c>
       <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2299,6 +3343,11 @@
         </is>
       </c>
       <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2325,6 +3374,11 @@
         </is>
       </c>
       <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2351,6 +3405,11 @@
         </is>
       </c>
       <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2377,6 +3436,11 @@
         </is>
       </c>
       <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2403,6 +3467,11 @@
         </is>
       </c>
       <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2429,6 +3498,11 @@
         </is>
       </c>
       <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2455,6 +3529,11 @@
         </is>
       </c>
       <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2481,6 +3560,11 @@
         </is>
       </c>
       <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2507,6 +3591,11 @@
         </is>
       </c>
       <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2533,6 +3622,11 @@
         </is>
       </c>
       <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2559,6 +3653,11 @@
         </is>
       </c>
       <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2584,7 +3683,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr">
+      <c r="F76" t="n">
+        <v>1</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>{"L3":1}</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>{"L3":1.0}</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -2614,7 +3734,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr">
+      <c r="F77" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>{"L2":1}</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>{"L2":1.0}</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>1</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>100.00</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
         <is>
           <t>L2</t>
         </is>
@@ -2644,7 +3785,28 @@
           <t>1</t>
         </is>
       </c>
-      <c r="F78" t="inlineStr">
+      <c r="F78" t="n">
+        <v>9</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>{"L3":8,"L1":1}</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>{"L3":0.8888888889,"L1":0.1111111111}</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>88.89</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
         <is>
           <t>L3</t>
         </is>
@@ -2675,6 +3837,11 @@
         </is>
       </c>
       <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2701,6 +3868,11 @@
         </is>
       </c>
       <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2727,6 +3899,11 @@
         </is>
       </c>
       <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2753,6 +3930,11 @@
         </is>
       </c>
       <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2779,6 +3961,11 @@
         </is>
       </c>
       <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2805,6 +3992,11 @@
         </is>
       </c>
       <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2831,6 +4023,11 @@
         </is>
       </c>
       <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2857,6 +4054,11 @@
         </is>
       </c>
       <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2883,6 +4085,11 @@
         </is>
       </c>
       <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
+      <c r="K87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2909,6 +4116,11 @@
         </is>
       </c>
       <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -2935,6 +4147,11 @@
         </is>
       </c>
       <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2961,6 +4178,11 @@
         </is>
       </c>
       <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
+      <c r="K90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -2987,6 +4209,11 @@
         </is>
       </c>
       <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -3013,6 +4240,11 @@
         </is>
       </c>
       <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
+      <c r="K92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -3039,6 +4271,11 @@
         </is>
       </c>
       <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -3065,6 +4302,11 @@
         </is>
       </c>
       <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
+      <c r="K94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -3091,6 +4333,11 @@
         </is>
       </c>
       <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -3117,6 +4364,11 @@
         </is>
       </c>
       <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
+      <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
+      <c r="K96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -3143,6 +4395,11 @@
         </is>
       </c>
       <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
+      <c r="K97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -3169,6 +4426,11 @@
         </is>
       </c>
       <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
+      <c r="K98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -3195,6 +4457,11 @@
         </is>
       </c>
       <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -3221,6 +4488,11 @@
         </is>
       </c>
       <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -3247,6 +4519,11 @@
         </is>
       </c>
       <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -3273,6 +4550,11 @@
         </is>
       </c>
       <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>